<commit_message>
No results screen added
</commit_message>
<xml_diff>
--- a/Documentación/Tiempo.xlsx
+++ b/Documentación/Tiempo.xlsx
@@ -550,7 +550,7 @@
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -678,7 +678,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="3">
         <f>SUM(E3:E14)</f>
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fallo con la validación de la clase ATermUtils
</commit_message>
<xml_diff>
--- a/Documentación/Tiempo.xlsx
+++ b/Documentación/Tiempo.xlsx
@@ -550,7 +550,7 @@
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="2">
-        <v>16.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -678,7 +678,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="3">
         <f>SUM(E3:E14)</f>
-        <v>101.5</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
La clasificación del razonador empieza en una asynctask
</commit_message>
<xml_diff>
--- a/Documentación/Tiempo.xlsx
+++ b/Documentación/Tiempo.xlsx
@@ -550,7 +550,7 @@
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="2">
-        <v>16.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -678,7 +678,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="3">
         <f>SUM(E3:E14)</f>
-        <v>101.5</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
App funcionando contra el server
</commit_message>
<xml_diff>
--- a/Documentación/Tiempo.xlsx
+++ b/Documentación/Tiempo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferzi\Documents\Univesidad\TFG\BeerAdvicer\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferzi\Documents\Univesidad\TFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -617,7 +617,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="2">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -678,7 +678,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="3">
         <f>SUM(E3:E14)</f>
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>